<commit_message>
[master] Add aulas de preprocessing e novas listas
</commit_message>
<xml_diff>
--- a/aulas/preprocessing/db_aulas/PI_Mestrado/Cronograma.xlsx
+++ b/aulas/preprocessing/db_aulas/PI_Mestrado/Cronograma.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Processamento de Imagens - Semestre 2018.1 (Turma INF, Prof. Filipe Cordeiro)</t>
   </si>
@@ -25,37 +25,52 @@
     <t>Estudo</t>
   </si>
   <si>
+    <t>Obs</t>
+  </si>
+  <si>
     <t>Capítulo 1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lista 1</t>
+    <t xml:space="preserve"> Lista Cap 1</t>
   </si>
   <si>
     <t>Capítulo 2:  Fundamentos de Imagens Digital</t>
   </si>
   <si>
-    <t>Lista 2</t>
+    <t>Lista Cap 2</t>
   </si>
   <si>
     <t>Capítulo 3:  Transformações de Intensidade e Filtragem Espacial</t>
   </si>
   <si>
-    <t>Lista 3</t>
+    <t>Lista Cap 3</t>
   </si>
   <si>
     <t>Capítulo 4: Filtragem no Domínio da Frequência</t>
   </si>
   <si>
+    <t>Deixei um slide do Prof. Valmir, para esse capítulo, no drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer um resumo (min 4 pgs) do Cap. 4 (seções 4.1, 4.5.5, 4.7, 4.8, 4.9.0 até 4.9.5 </t>
+  </si>
+  <si>
+    <t>Capítulo 5: Restauração e reconstrução de imagens</t>
+  </si>
+  <si>
+    <t>Lista Cap 5</t>
+  </si>
+  <si>
+    <t>Capítulo 6: Processamento de imagens coloridas</t>
+  </si>
+  <si>
+    <t>Lista Cap 6</t>
+  </si>
+  <si>
+    <t>Capítulo 7: Processamento com wavelets e multirresolução</t>
+  </si>
+  <si>
     <t>ainda não divulgado</t>
-  </si>
-  <si>
-    <t>Capítulo 5: Restauração e reconstrução de imagens</t>
-  </si>
-  <si>
-    <t>Capítulo 6: Processamento de imagens coloridas</t>
-  </si>
-  <si>
-    <t>Capítulo 7: Processamento com wavelets e multirresolução</t>
   </si>
   <si>
     <t>Capítulo 9: Processamento morfológico de imagens</t>
@@ -123,7 +138,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +149,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
@@ -272,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -293,39 +314,54 @@
     <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="4" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="4" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="3" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="4" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -335,7 +371,7 @@
     <xf borderId="10" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="4" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -365,7 +401,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.44"/>
-    <col customWidth="1" min="2" max="2" width="20.33"/>
+    <col customWidth="1" min="2" max="2" width="26.11"/>
     <col customWidth="1" min="3" max="3" width="61.33"/>
     <col customWidth="1" min="4" max="4" width="20.44"/>
     <col customWidth="1" min="5" max="26" width="10.56"/>
@@ -393,302 +429,309 @@
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>43210.0</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>43213.0</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <f t="shared" ref="A6:A34" si="1">A4+7</f>
         <v>43217</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="16">
+      <c r="A7" s="17">
         <f t="shared" si="1"/>
         <v>43220</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="17">
+      <c r="A8" s="18">
         <f t="shared" si="1"/>
         <v>43224</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="15"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="16">
+      <c r="A9" s="17">
         <f t="shared" si="1"/>
         <v>43227</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="17">
+      <c r="C9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" ht="33.0" customHeight="1">
+      <c r="A10" s="21">
         <f t="shared" si="1"/>
         <v>43231</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="16">
+      <c r="A11" s="23">
         <f t="shared" si="1"/>
         <v>43234</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>12</v>
+      <c r="B11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="17">
+      <c r="A12" s="18">
         <f t="shared" si="1"/>
         <v>43238</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="16">
+      <c r="A13" s="17">
         <f t="shared" si="1"/>
         <v>43241</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>13</v>
+      <c r="B13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="17">
+      <c r="A14" s="18">
         <f t="shared" si="1"/>
         <v>43245</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="16">
+      <c r="A15" s="17">
         <f t="shared" si="1"/>
         <v>43248</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>14</v>
+      <c r="B15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="17">
+      <c r="A16" s="18">
         <f t="shared" si="1"/>
         <v>43252</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="16">
+      <c r="A17" s="17">
         <f t="shared" si="1"/>
         <v>43255</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>15</v>
+      <c r="B17" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="17">
+      <c r="A18" s="18">
         <f t="shared" si="1"/>
         <v>43259</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="16">
+      <c r="A19" s="17">
         <f t="shared" si="1"/>
         <v>43262</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>16</v>
+      <c r="B19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="17">
+      <c r="A20" s="18">
         <f t="shared" si="1"/>
         <v>43266</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="16">
+      <c r="A21" s="17">
         <f t="shared" si="1"/>
         <v>43269</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>17</v>
+      <c r="B21" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="17">
+      <c r="A22" s="18">
         <f t="shared" si="1"/>
         <v>43273</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="16">
+      <c r="A23" s="17">
         <f t="shared" si="1"/>
         <v>43276</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>18</v>
+      <c r="B23" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="17">
+      <c r="A24" s="18">
         <f t="shared" si="1"/>
         <v>43280</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="15"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="16">
+      <c r="A25" s="17">
         <f t="shared" si="1"/>
         <v>43283</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>20</v>
+      <c r="B25" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="17">
+      <c r="A26" s="18">
         <f t="shared" si="1"/>
         <v>43287</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="22"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="23">
+      <c r="A27" s="28">
         <f t="shared" si="1"/>
         <v>43290</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="17">
+      <c r="A28" s="18">
         <f t="shared" si="1"/>
         <v>43294</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="23">
+      <c r="A29" s="28">
         <f t="shared" si="1"/>
         <v>43297</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="27"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="17">
+      <c r="A30" s="18">
         <f t="shared" si="1"/>
         <v>43301</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="27"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="17">
+      <c r="A31" s="18">
         <f t="shared" si="1"/>
         <v>43304</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="22"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="27"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="17">
+      <c r="A32" s="18">
         <f t="shared" si="1"/>
         <v>43308</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="15"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="24">
+      <c r="A33" s="29">
         <f t="shared" si="1"/>
         <v>43311</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>22</v>
+      <c r="B33" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="17">
+      <c r="A34" s="18">
         <f t="shared" si="1"/>
         <v>43315</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="9" t="s">
-        <v>23</v>
+      <c r="B34" s="19"/>
+      <c r="C34" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1658,10 +1701,11 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>

</xml_diff>

<commit_message>
[master] Aulas de preprocessamento final
</commit_message>
<xml_diff>
--- a/aulas/preprocessing/db_aulas/PI_Mestrado/Cronograma.xlsx
+++ b/aulas/preprocessing/db_aulas/PI_Mestrado/Cronograma.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Processamento de Imagens - Semestre 2018.1 (Turma INF, Prof. Filipe Cordeiro)</t>
   </si>
@@ -70,16 +70,25 @@
     <t>Capítulo 7: Processamento com wavelets e multirresolução</t>
   </si>
   <si>
-    <t>ainda não divulgado</t>
+    <t>Fazer um resumo (min 3 pgs) do Cap. 7 (seções 7.1, 7.5)</t>
   </si>
   <si>
     <t>Capítulo 9: Processamento morfológico de imagens</t>
   </si>
   <si>
+    <t>Lista Cap 9</t>
+  </si>
+  <si>
     <t>Capítulo 10: Segmentação de imagens</t>
   </si>
   <si>
+    <t>Lista Cap 10</t>
+  </si>
+  <si>
     <t>Capítulo 11: representação e descrição</t>
+  </si>
+  <si>
+    <t>Lista Cap 11</t>
   </si>
   <si>
     <t>Capítulo 12: Reconhecimento de Objetos</t>
@@ -569,7 +578,7 @@
         <f t="shared" si="1"/>
         <v>43255</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -589,11 +598,11 @@
         <f t="shared" si="1"/>
         <v>43262</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>19</v>
+      <c r="B19" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -609,11 +618,11 @@
         <f t="shared" si="1"/>
         <v>43269</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>19</v>
+      <c r="B21" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -629,11 +638,11 @@
         <f t="shared" si="1"/>
         <v>43276</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>19</v>
+      <c r="B23" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -650,10 +659,10 @@
         <v>43283</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -718,10 +727,10 @@
         <v>43311</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -731,7 +740,7 @@
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>